<commit_message>
falta hacer validacion del llenado de indicadores
</commit_message>
<xml_diff>
--- a/public/img/plantilla.xlsx
+++ b/public/img/plantilla.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desar\Desktop\balanced\public\img\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36368D29-8ACB-499D-9493-76CE2FD5327E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="4350" yWindow="4140" windowWidth="23775" windowHeight="10170" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,26 +27,23 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve">id</t>
+    <t>id</t>
   </si>
   <si>
-    <t xml:space="preserve">Nombre</t>
+    <t>nombre</t>
   </si>
   <si>
-    <t xml:space="preserve">Descripción</t>
+    <t>descripcion</t>
   </si>
   <si>
-    <t xml:space="preserve">Información</t>
+    <t>informacion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,22 +52,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -82,74 +69,52 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.5"/>
+        <fgColor theme="4" tint="-0.499984740745262"/>
         <bgColor rgb="FF003366"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -208,60 +173,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF1F4E79"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -293,7 +274,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -317,7 +298,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -377,31 +358,30 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="30.71"/>
+    <col min="1" max="4" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -415,277 +395,272 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>